<commit_message>
changes in cater excwl
</commit_message>
<xml_diff>
--- a/back-end/CaterBackend/dataregardCater2.xlsx
+++ b/back-end/CaterBackend/dataregardCater2.xlsx
@@ -1,22 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4794CF4-7B25-481C-BF9D-EB8AADA5672D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>https://image.wedmegood.com/resized/450X/uploads/member/2217715/1627736739_IMG_20210715_101647.jpg?crop=315,0,1641,923</t>
   </si>
@@ -94,23 +87,209 @@
     <t>loginUserId</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>dev@gmail.com</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
-    <t>indore</t>
+    <t>Culinary Odyssey</t>
+  </si>
+  <si>
+    <t>Tasteful Trends</t>
+  </si>
+  <si>
+    <t>Epicurean Escapes</t>
+  </si>
+  <si>
+    <t>Palate Pleasers</t>
+  </si>
+  <si>
+    <t>Gastronomic Delights</t>
+  </si>
+  <si>
+    <t>Savory Soirees</t>
+  </si>
+  <si>
+    <t>Flavor Fusion</t>
+  </si>
+  <si>
+    <t>Culinary Chronicle</t>
+  </si>
+  <si>
+    <t>Gourmet Gala</t>
+  </si>
+  <si>
+    <t>Delectable Affairs</t>
+  </si>
+  <si>
+    <t>CaterJoy</t>
+  </si>
+  <si>
+    <t>Bite Bliss Catering</t>
+  </si>
+  <si>
+    <t>Feast Fables</t>
+  </si>
+  <si>
+    <t>Culinary Carousel</t>
+  </si>
+  <si>
+    <t>Savvy Sustenance</t>
+  </si>
+  <si>
+    <t>Banquet Bonanza</t>
+  </si>
+  <si>
+    <t>Tantalizing Tastings</t>
+  </si>
+  <si>
+    <t>Nosh Nectar</t>
+  </si>
+  <si>
+    <t>Gourmet Gaiety</t>
+  </si>
+  <si>
+    <t>Epic Eats Events</t>
+  </si>
+  <si>
+    <t>Elite Eats Catering</t>
+  </si>
+  <si>
+    <t>Culinary Craftsmen</t>
+  </si>
+  <si>
+    <t>Epicurean Excellence</t>
+  </si>
+  <si>
+    <t>Gourmet Gurus</t>
+  </si>
+  <si>
+    <t>vijay nagar Indore</t>
+  </si>
+  <si>
+    <t>Bhawarkua, Indore</t>
+  </si>
+  <si>
+    <t>Rajwada, Indore</t>
+  </si>
+  <si>
+    <t>Palasia, Indore</t>
+  </si>
+  <si>
+    <t>Tilak Nagar, Indore</t>
+  </si>
+  <si>
+    <t>Sudama Nagar, Indore</t>
+  </si>
+  <si>
+    <t>Pardesipura, Indore</t>
+  </si>
+  <si>
+    <t>Bengali Square, Indore</t>
+  </si>
+  <si>
+    <t>Rau, Indore</t>
+  </si>
+  <si>
+    <t>MR 10 Road, Indore</t>
+  </si>
+  <si>
+    <t>Mahalaxmi Nagar, Indore</t>
+  </si>
+  <si>
+    <t>Navlakha, Indore</t>
+  </si>
+  <si>
+    <t>Annapurna, Indore</t>
+  </si>
+  <si>
+    <t>Lokmanya Nagar, Indore</t>
+  </si>
+  <si>
+    <t>Snehnagar, Indore</t>
+  </si>
+  <si>
+    <t>Scheme No. 54, Indore</t>
+  </si>
+  <si>
+    <t>Scheme No. 74, Indore</t>
+  </si>
+  <si>
+    <t>Sukhliya, Indore</t>
+  </si>
+  <si>
+    <t>Nipania, Indore</t>
+  </si>
+  <si>
+    <t>Airport Road, Indore</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT9DZ3q19LSL6y0ayUtWU7wG3MVXKWpBohYjw&amp;s</t>
+  </si>
+  <si>
+    <t>https://assets-global.website-files.com/563a58ee6b1ce88d50f9edde/62e03021a85da51781953976_catering-team-02.jpeg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTvY_I27xPbKCzoOiO5Klo0YHXHShjQkp8CVQ&amp;s</t>
+  </si>
+  <si>
+    <t>https://d3jmn01ri1fzgl.cloudfront.net/photoadking/webp_thumbnail/catering-service-flyer-template-cn5uz1194d3a82.webp</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQNwQLxBxe4uS54as8HTVOphGSzzFot-hr3gw&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcS-8C3P06jH4Gjr5tlVWTLIU3eZ0ZqpxPGdTw&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTmMKb7BWk0Kc2yO5LoTtgiuMrCJGy-wL1y1w&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT3j2M7-qqbYmt_LqzE9R5sE7i5SazA_CjCWA&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTaKOm5W_ASDmttiE3VY2gCvPq3fmLIfFBpEQ&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTZo849grNkMn_pMLEGBNKj42DA63lj16q3wg&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRX61ualMdz5yI3e3emBDw_vv5pgBMNdpAC5A&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTttFnw1ys7eNRV9jX2KshPWEEf6qpPL9RQFA&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTwklrfHG9YcR9GifQBT3BEWMceGWoOZRsmug&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTtEZZEm7Ugb7AQbdtFiZ6I3Q1SBrAhvFKYxQ&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTzsjmMnIVqAYzSIIohSV1a-S3SfDlkzJ5yXg&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR9u66cLknS0oEmCOGftgcfpRT1JvCBn1Fb1A&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTeGY7qMlOy1U83qnb4fWWHEQbn0oYDwb2yIg&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcS4fIW2DOwsHLLjJOR93ZuVraOrzz7XpDHMmA&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ2P6eJeNXsXnFqPXsxFFBxdUeakuoUEWNnJQ&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSlG7I31Jx2v0AVOM3JkTDenVDxMtpWlhM74Q&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcScjJrZGl6MMoaqsgCIcntOXng2GrcEb6fc6A&amp;s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,12 +298,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Var(--ricos-custom-p-font-famil"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,11 +326,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -159,12 +340,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -181,9 +360,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,7 +400,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -255,7 +434,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -290,10 +468,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,24 +643,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="131" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
     <col min="10" max="10" width="47.88671875" customWidth="1"/>
     <col min="11" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -496,20 +677,18 @@
       <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="18" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -520,23 +699,21 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>20000</v>
+      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3">
         <v>9789596548</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18" customHeight="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -547,23 +724,21 @@
         <v>3</v>
       </c>
       <c r="D3" s="2">
-        <v>100</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>25000</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3">
         <v>9789596548</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="18" customHeight="1">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -574,23 +749,21 @@
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>100</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>30000</v>
+      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3">
         <v>9789596548</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="18" customHeight="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -601,23 +774,21 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>100</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>35000</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3">
         <v>9789596548</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="18" customHeight="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -628,23 +799,21 @@
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <v>100</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>40000</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3">
         <v>9789596548</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="18" customHeight="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -655,23 +824,21 @@
         <v>11</v>
       </c>
       <c r="D7" s="2">
-        <v>100</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>45000</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3">
         <v>9789596548</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="18" customHeight="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -682,33 +849,598 @@
         <v>13</v>
       </c>
       <c r="D8" s="2">
-        <v>100</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>50000</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3">
         <v>9789596548</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L8" s="1"/>
     </row>
+    <row r="9" spans="1:12" ht="18" customHeight="1">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2">
+        <v>55000</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18" customHeight="1">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="18" customHeight="1">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2">
+        <v>65000</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18" customHeight="1">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2">
+        <v>70000</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2">
+        <v>75000</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2">
+        <v>80000</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18" customHeight="1">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2">
+        <v>85000</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" customHeight="1">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2">
+        <v>90000</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2">
+        <v>95000</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="2">
+        <v>105000</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18" customHeight="1">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2">
+        <v>110000</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" customHeight="1">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="2">
+        <v>115000</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" customHeight="1">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2">
+        <v>120000</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18" customHeight="1">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="2">
+        <v>125000</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" customHeight="1">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="2">
+        <v>130000</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18" customHeight="1">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>24</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="2">
+        <v>135000</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18" customHeight="1">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2">
+        <v>140000</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" customHeight="1">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3">
+        <v>26</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="2">
+        <v>145000</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" customHeight="1">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2">
+        <v>150000</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18" customHeight="1">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
+        <v>28</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="2">
+        <v>155000</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" customHeight="1">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>29</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="2">
+        <v>160000</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" customHeight="1">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="2">
+        <v>165000</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" customHeight="1">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>31</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="2">
+        <v>170000</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>9789596548</v>
+      </c>
+      <c r="G32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{35DFD3EC-60D3-49FE-9036-27D750C7EED3}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{CBC08277-D16C-4AD5-BBAF-E316266D5669}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{8E3FF504-3D29-401C-AF24-0889E7CED09F}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{4DB0327E-86D7-49B9-B3E7-63EED3EC58CC}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{23E65B25-DCF0-47E3-A9A2-0657A49ACEC2}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{0E034A60-7041-49F4-9B5D-8E11364259A6}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{B676F791-6C5A-43FC-AF83-B720120C2288}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>